<commit_message>
latest sync from latop
</commit_message>
<xml_diff>
--- a/budget/sonikebanaV2_budget.xlsx
+++ b/budget/sonikebanaV2_budget.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mparker/Dropbox/pieces/Sonikebana/version2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mparker/Dropbox/pieces/sonikebana/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5F037E-8D27-8341-8162-098B7B0EA853}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A00224-3A8E-3A47-B70A-FAC4DCDF8074}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{428476F3-695E-A64D-B0F7-882B1B92CFAA}"/>
+    <workbookView xWindow="680" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{428476F3-695E-A64D-B0F7-882B1B92CFAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Calculations for Wood" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Wood for speakers</t>
   </si>
@@ -69,9 +70,6 @@
     <t>Large, custom cushion for westcourt and future concerts</t>
   </si>
   <si>
-    <t>3ply white</t>
-  </si>
-  <si>
     <t>standard latest computers</t>
   </si>
   <si>
@@ -103,6 +101,57 @@
   </si>
   <si>
     <t>Amplifier and pi DAC</t>
+  </si>
+  <si>
+    <t>SD cards for RpI</t>
+  </si>
+  <si>
+    <t>Tops and bottoms</t>
+  </si>
+  <si>
+    <t>Heights</t>
+  </si>
+  <si>
+    <t>38*38 softwood</t>
+  </si>
+  <si>
+    <t>12mm birch ply</t>
+  </si>
+  <si>
+    <t>Wood beams</t>
+  </si>
+  <si>
+    <t>MDF for bases</t>
+  </si>
+  <si>
+    <t>MDF bases</t>
+  </si>
+  <si>
+    <t>sticks</t>
+  </si>
+  <si>
+    <t>1200*2440*12mm Birch Ply</t>
+  </si>
+  <si>
+    <t>VAT excl</t>
+  </si>
+  <si>
+    <t>Vat Incl</t>
+  </si>
+  <si>
+    <t>1200*2440*12mm MDF</t>
+  </si>
+  <si>
+    <t>38*50mm softwood, price per meter</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt; price per meter, length can be division of the 4.8m lengths. </t>
+  </si>
+  <si>
+    <t>printing onto boxes</t>
   </si>
 </sst>
 </file>
@@ -460,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D5B1481-BDB9-DD4A-AB9A-B0FD0DED0F1B}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,11 +533,11 @@
         <v>-65</v>
       </c>
       <c r="C1">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2">
-        <f t="shared" ref="D1:D17" si="0">B1*C1</f>
-        <v>-1105</v>
+        <f t="shared" ref="D1:D21" si="0">B1*C1</f>
+        <v>-585</v>
       </c>
       <c r="E1" t="s">
         <v>12</v>
@@ -499,269 +548,762 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>-50</v>
+        <v>-41.64</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2">
         <f t="shared" si="0"/>
-        <v>-450</v>
+        <v>-582.96</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2">
-        <v>-35</v>
+        <v>-1.34</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" si="0"/>
-        <v>-315</v>
+        <f>B3*C3</f>
+        <v>-120.60000000000001</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2">
-        <v>-300</v>
+        <v>-17.5</v>
       </c>
       <c r="C4">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" si="0"/>
-        <v>-2700</v>
+        <f>B4*C4</f>
+        <v>-87.5</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" s="2">
-        <v>-42</v>
+        <v>-35</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-315</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
-        <v>-20</v>
+        <v>-260</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2340</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="B7" s="2">
-        <v>-10</v>
+        <v>-534</v>
       </c>
       <c r="C7">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>-90</v>
+        <v>-534</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" s="2">
-        <v>-15</v>
+        <v>-42</v>
       </c>
       <c r="C8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>-135</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2">
-        <v>-45</v>
+        <v>-20</v>
       </c>
       <c r="C9">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>-405</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2">
-        <v>-62</v>
+        <v>-5.37</v>
       </c>
       <c r="C10">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>-620</v>
+        <v>-193.32</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2">
-        <v>-60</v>
+        <v>-10</v>
       </c>
       <c r="C11">
         <v>9</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>-540</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2">
-        <v>-100</v>
+        <v>-15</v>
       </c>
       <c r="C12">
         <v>9</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>-900</v>
+        <v>-135</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B13" s="2">
-        <v>-15</v>
+        <v>-45</v>
       </c>
       <c r="C13">
         <v>9</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>-135</v>
+        <v>-405</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2">
+        <v>-62</v>
+      </c>
+      <c r="C14">
         <v>10</v>
       </c>
-      <c r="B14" s="2">
-        <v>-450</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>-450</v>
-      </c>
-      <c r="E14" t="s">
-        <v>20</v>
+        <v>-620</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2">
-        <v>-45</v>
+        <v>-60</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>-90</v>
-      </c>
-      <c r="E15" t="s">
-        <v>19</v>
+        <v>-540</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2">
-        <v>-250</v>
+        <v>-100</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>-500</v>
-      </c>
-      <c r="E16" t="s">
-        <v>23</v>
+        <v>-900</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2">
+        <v>-15</v>
+      </c>
+      <c r="C17">
+        <v>9</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>-135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2">
+        <v>-450</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>-450</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2">
+        <v>-45</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>-90</v>
+      </c>
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2">
+        <v>-350</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>-700</v>
+      </c>
+      <c r="E20" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="2">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="2">
         <v>-450</v>
       </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2">
+        <f>SUM(D$1:D$23)</f>
+        <v>-8823.3799999999992</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{944D7162-D4F3-4F42-8D77-8F6AFD16FA7E}">
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:F37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1700</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <f>A2*B2</f>
+        <v>6800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1000</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C28" si="0">A3*B3</f>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>600</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>450</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>600</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>450</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1500</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>800</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>850</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>470</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1200</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1000</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1200</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1000</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>850</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>470</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
       <c r="C17">
+        <f t="shared" si="0"/>
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>600</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>450</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>450</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>800</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>800</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>800</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>600</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>600</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>450</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <f>SUM(C2:C28)</f>
+        <v>78760</v>
+      </c>
+      <c r="D31">
+        <f>C31/1000</f>
+        <v>78.760000000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>1</v>
       </c>
-      <c r="D17" s="2">
-        <f t="shared" si="0"/>
-        <v>-450</v>
-      </c>
-      <c r="E17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="D34">
+        <f>C34*1.2</f>
+        <v>41.64</v>
+      </c>
+      <c r="E34">
+        <v>14</v>
+      </c>
+      <c r="F34">
+        <f>E34*D34</f>
+        <v>582.96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35">
         <v>2</v>
       </c>
-      <c r="D20" s="2">
-        <f>SUM(D$1:D$19)</f>
-        <v>-8885</v>
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35">
+        <v>14.54</v>
+      </c>
+      <c r="D35">
+        <f>C35*1.2</f>
+        <v>17.447999999999997</v>
+      </c>
+      <c r="E35">
+        <v>5</v>
+      </c>
+      <c r="F35">
+        <f>E35*D35</f>
+        <v>87.239999999999981</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36">
+        <v>0.73</v>
+      </c>
+      <c r="D36">
+        <f>C36*1.2</f>
+        <v>0.876</v>
+      </c>
+      <c r="E36">
+        <v>80</v>
+      </c>
+      <c r="F36">
+        <f>E36*D36</f>
+        <v>70.08</v>
+      </c>
+      <c r="G36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E37" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37">
+        <f>SUM(F34:F36)</f>
+        <v>740.28000000000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>